<commit_message>
threads, gonna use for my linux?
</commit_message>
<xml_diff>
--- a/db/balancing/balancing.xlsx
+++ b/db/balancing/balancing.xlsx
@@ -4158,8 +4158,8 @@
   <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8523,22 +8523,22 @@
         <v>1</v>
       </c>
       <c r="J74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O74" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P74" s="2">
         <v>0</v>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="T74" s="3">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>